<commit_message>
Change the project title and label in the new SS2 spreadsheets (without accessions)
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/current/not_accessioned_dcp_integration_test_metadata_1_SS2_bundle.xlsx
+++ b/infrastructure_testing_files/current/not_accessioned_dcp_integration_test_metadata_1_SS2_bundle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karoly/dev/hca/metadata-schema/infrastructure_testing_files/current/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D656BAD9-3776-FC47-B8B6-CA4DF546920D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D224BAC-26DE-8544-A6DA-CD2F3478372D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="-4660" windowWidth="51200" windowHeight="21940" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-51200" yWindow="-5780" windowWidth="51200" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -1647,9 +1647,6 @@
     <t>SEQUENCING_PROTOCOL.SEQUENCING_APPROACH.ONTOLOGY_LABEL</t>
   </si>
   <si>
-    <t>SS2 1 Cell Integration Test</t>
-  </si>
-  <si>
     <t>https://github.com/czbiohub/tabula-muris; http://celltag.org/</t>
   </si>
   <si>
@@ -2275,6 +2272,9 @@
   </si>
   <si>
     <t>HsapDv:0000087</t>
+  </si>
+  <si>
+    <t>SS2 1 Cell Integration Test without accessions</t>
   </si>
 </sst>
 </file>
@@ -2675,8 +2675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2752,7 +2752,7 @@
         <v>15</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>21</v>
@@ -2761,7 +2761,7 @@
         <v>24</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -2778,16 +2778,16 @@
         <v>16</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>667</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>668</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>669</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>670</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>671</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -2804,16 +2804,16 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>744</v>
+      </c>
+      <c r="B6" t="s">
+        <v>744</v>
+      </c>
+      <c r="C6" t="s">
+        <v>536</v>
+      </c>
+      <c r="D6" t="s">
         <v>535</v>
-      </c>
-      <c r="B6" t="s">
-        <v>535</v>
-      </c>
-      <c r="C6" t="s">
-        <v>537</v>
-      </c>
-      <c r="D6" t="s">
-        <v>536</v>
       </c>
     </row>
   </sheetData>
@@ -2944,13 +2944,13 @@
         <v>412</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>688</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>689</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>690</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>691</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -2968,31 +2968,31 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B6" t="s">
+        <v>623</v>
+      </c>
+      <c r="C6" t="s">
         <v>624</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>618</v>
+      </c>
+      <c r="E6" t="s">
+        <v>619</v>
+      </c>
+      <c r="F6" t="s">
+        <v>620</v>
+      </c>
+      <c r="G6" t="s">
+        <v>627</v>
+      </c>
+      <c r="H6" t="s">
         <v>625</v>
       </c>
-      <c r="D6" t="s">
-        <v>619</v>
-      </c>
-      <c r="E6" t="s">
-        <v>620</v>
-      </c>
-      <c r="F6" t="s">
-        <v>621</v>
-      </c>
-      <c r="G6" t="s">
-        <v>628</v>
-      </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>626</v>
-      </c>
-      <c r="I6" t="s">
-        <v>627</v>
       </c>
     </row>
   </sheetData>
@@ -3151,22 +3151,22 @@
         <v>421</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>707</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>708</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>709</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>710</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>428</v>
       </c>
       <c r="K4" s="3" t="s">
+        <v>710</v>
+      </c>
+      <c r="L4" s="3" t="s">
         <v>711</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>712</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3187,34 +3187,34 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>629</v>
+      </c>
+      <c r="B6" t="s">
         <v>630</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>631</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>618</v>
+      </c>
+      <c r="E6" t="s">
+        <v>619</v>
+      </c>
+      <c r="F6" t="s">
+        <v>620</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>633</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>634</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>635</v>
+      </c>
+      <c r="J6" t="s">
         <v>632</v>
-      </c>
-      <c r="D6" t="s">
-        <v>619</v>
-      </c>
-      <c r="E6" t="s">
-        <v>620</v>
-      </c>
-      <c r="F6" t="s">
-        <v>621</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>634</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>635</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>636</v>
-      </c>
-      <c r="J6" t="s">
-        <v>633</v>
       </c>
       <c r="K6">
         <v>70</v>
@@ -3232,7 +3232,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:AF6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
@@ -3295,13 +3295,13 @@
         <v>463</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>676</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>677</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>678</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>468</v>
@@ -3589,13 +3589,13 @@
         <v>466</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="R4" s="3" t="s">
         <v>471</v>
@@ -3681,84 +3681,84 @@
     </row>
     <row r="6" spans="1:32" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>636</v>
+      </c>
+      <c r="B6" t="s">
+        <v>638</v>
+      </c>
+      <c r="C6" t="s">
         <v>637</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
+        <v>618</v>
+      </c>
+      <c r="E6" t="s">
+        <v>619</v>
+      </c>
+      <c r="F6" t="s">
+        <v>620</v>
+      </c>
+      <c r="K6" s="3" t="s">
         <v>639</v>
       </c>
-      <c r="C6" t="s">
-        <v>638</v>
-      </c>
-      <c r="D6" t="s">
-        <v>619</v>
-      </c>
-      <c r="E6" t="s">
-        <v>620</v>
-      </c>
-      <c r="F6" t="s">
-        <v>621</v>
-      </c>
-      <c r="K6" s="3" t="s">
+      <c r="L6" s="3" t="s">
         <v>640</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="M6" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="N6" s="3" t="s">
         <v>641</v>
       </c>
-      <c r="M6" s="3" t="s">
-        <v>640</v>
-      </c>
-      <c r="N6" s="3" t="s">
+      <c r="O6" s="3" t="s">
         <v>642</v>
       </c>
-      <c r="O6" s="3" t="s">
+      <c r="P6" s="3" t="s">
         <v>643</v>
       </c>
-      <c r="P6" s="3" t="s">
+      <c r="Q6" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="R6" s="3" t="s">
         <v>644</v>
-      </c>
-      <c r="Q6" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>645</v>
       </c>
       <c r="S6">
         <v>20014279</v>
       </c>
       <c r="T6" s="3" t="s">
+        <v>645</v>
+      </c>
+      <c r="U6" t="s">
         <v>646</v>
-      </c>
-      <c r="U6" t="s">
-        <v>647</v>
       </c>
       <c r="V6" s="7"/>
       <c r="W6" t="s">
+        <v>647</v>
+      </c>
+      <c r="X6" t="s">
         <v>648</v>
-      </c>
-      <c r="X6" t="s">
-        <v>649</v>
       </c>
       <c r="Y6">
         <v>20014279</v>
       </c>
       <c r="Z6" t="s">
+        <v>645</v>
+      </c>
+      <c r="AA6" t="s">
         <v>646</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>647</v>
       </c>
       <c r="AB6" s="5"/>
       <c r="AC6" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="AD6" s="6" t="s">
+        <v>649</v>
+      </c>
+      <c r="AE6" s="3" t="s">
         <v>650</v>
       </c>
-      <c r="AE6" s="3" t="s">
+      <c r="AF6" s="3" t="s">
         <v>651</v>
-      </c>
-      <c r="AF6" s="3" t="s">
-        <v>652</v>
       </c>
     </row>
   </sheetData>
@@ -3953,13 +3953,13 @@
         <v>530</v>
       </c>
       <c r="L4" s="3" t="s">
+        <v>691</v>
+      </c>
+      <c r="M4" s="3" t="s">
         <v>692</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>693</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>694</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3982,46 +3982,46 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B6" t="s">
+        <v>652</v>
+      </c>
+      <c r="C6" t="s">
         <v>653</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>618</v>
+      </c>
+      <c r="E6" t="s">
+        <v>619</v>
+      </c>
+      <c r="F6" t="s">
+        <v>620</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>654</v>
       </c>
-      <c r="D6" t="s">
-        <v>619</v>
-      </c>
-      <c r="E6" t="s">
-        <v>620</v>
-      </c>
-      <c r="F6" t="s">
-        <v>621</v>
-      </c>
-      <c r="G6" s="3" t="s">
+      <c r="H6" s="3" t="s">
         <v>655</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="I6" s="3" t="s">
+        <v>654</v>
+      </c>
+      <c r="J6" t="s">
         <v>656</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>655</v>
-      </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
+        <v>550</v>
+      </c>
+      <c r="L6" s="3" t="s">
         <v>657</v>
       </c>
-      <c r="K6" t="s">
-        <v>551</v>
-      </c>
-      <c r="L6" s="3" t="s">
+      <c r="M6" s="3" t="s">
         <v>658</v>
       </c>
-      <c r="M6" s="3" t="s">
-        <v>659</v>
-      </c>
       <c r="N6" s="3" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
   </sheetData>
@@ -4142,7 +4142,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>33</v>
@@ -4166,7 +4166,7 @@
         <v>57</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>64</v>
@@ -4188,66 +4188,66 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B6" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C6" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="D6" t="s">
+        <v>544</v>
+      </c>
+      <c r="E6" t="s">
         <v>545</v>
       </c>
-      <c r="E6" t="s">
-        <v>546</v>
-      </c>
       <c r="F6" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="G6" t="s">
+        <v>549</v>
+      </c>
+      <c r="H6" t="s">
         <v>550</v>
       </c>
-      <c r="H6" t="s">
-        <v>551</v>
-      </c>
       <c r="I6" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="J6" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C7" t="s">
+        <v>542</v>
+      </c>
+      <c r="D7" t="s">
         <v>543</v>
       </c>
-      <c r="D7" t="s">
-        <v>544</v>
-      </c>
       <c r="E7" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="F7" t="s">
+        <v>548</v>
+      </c>
+      <c r="G7" t="s">
         <v>549</v>
       </c>
-      <c r="G7" t="s">
-        <v>550</v>
-      </c>
       <c r="H7" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="I7" t="s">
+        <v>553</v>
+      </c>
+      <c r="J7" t="s">
         <v>554</v>
-      </c>
-      <c r="J7" t="s">
-        <v>555</v>
       </c>
     </row>
   </sheetData>
@@ -4290,7 +4290,7 @@
         <v>80</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -4310,7 +4310,7 @@
         <v>81</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -4330,7 +4330,7 @@
         <v>82</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -4338,7 +4338,7 @@
         <v>68</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>75</v>
@@ -4347,10 +4347,10 @@
         <v>79</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4365,22 +4365,22 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>555</v>
+      </c>
+      <c r="B6" t="s">
         <v>556</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>557</v>
-      </c>
-      <c r="C6" t="s">
-        <v>558</v>
       </c>
       <c r="D6">
         <v>27565351</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="F6" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
   </sheetData>
@@ -4445,7 +4445,7 @@
         <v>90</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4457,13 +4457,13 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>559</v>
+      </c>
+      <c r="B6" t="s">
         <v>560</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>561</v>
-      </c>
-      <c r="C6" t="s">
-        <v>562</v>
       </c>
     </row>
   </sheetData>
@@ -4941,10 +4941,10 @@
         <v>113</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>701</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>702</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>703</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>123</v>
@@ -5105,115 +5105,115 @@
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>562</v>
+      </c>
+      <c r="B6" t="s">
         <v>563</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>564</v>
-      </c>
-      <c r="C6" t="s">
-        <v>565</v>
       </c>
       <c r="D6">
         <v>9606</v>
       </c>
       <c r="E6" t="s">
+        <v>565</v>
+      </c>
+      <c r="F6" t="s">
         <v>566</v>
-      </c>
-      <c r="F6" t="s">
-        <v>567</v>
       </c>
       <c r="I6">
         <v>36.4</v>
       </c>
       <c r="J6" s="3" t="s">
+        <v>567</v>
+      </c>
+      <c r="K6" s="3" t="s">
         <v>568</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="L6" s="3" t="s">
         <v>569</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="M6" s="3" t="s">
         <v>570</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="N6" s="3" t="s">
         <v>571</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="O6" s="3" t="s">
+        <v>570</v>
+      </c>
+      <c r="P6" t="s">
         <v>572</v>
       </c>
-      <c r="O6" s="3" t="s">
-        <v>571</v>
-      </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
+        <v>572</v>
+      </c>
+      <c r="R6" t="s">
         <v>573</v>
       </c>
-      <c r="Q6" t="s">
-        <v>573</v>
-      </c>
-      <c r="R6" t="s">
+      <c r="S6" s="3" t="s">
         <v>574</v>
       </c>
-      <c r="S6" s="3" t="s">
+      <c r="T6" s="3" t="s">
         <v>575</v>
       </c>
-      <c r="T6" s="3" t="s">
-        <v>576</v>
-      </c>
       <c r="U6" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="V6" t="s">
+        <v>742</v>
+      </c>
+      <c r="W6" t="s">
         <v>743</v>
       </c>
-      <c r="W6" t="s">
-        <v>744</v>
-      </c>
       <c r="X6" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="Y6" t="s">
+        <v>659</v>
+      </c>
+      <c r="Z6" t="s">
         <v>660</v>
       </c>
-      <c r="Z6" t="s">
-        <v>661</v>
-      </c>
       <c r="AA6" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="AB6">
         <v>22</v>
       </c>
       <c r="AC6" t="s">
+        <v>576</v>
+      </c>
+      <c r="AD6" s="3" t="s">
         <v>577</v>
       </c>
-      <c r="AD6" s="3" t="s">
+      <c r="AE6" t="s">
         <v>578</v>
-      </c>
-      <c r="AE6" t="s">
-        <v>579</v>
       </c>
       <c r="AF6">
         <v>160</v>
       </c>
       <c r="AG6" t="s">
+        <v>579</v>
+      </c>
+      <c r="AH6" t="s">
         <v>580</v>
       </c>
-      <c r="AH6" t="s">
-        <v>581</v>
-      </c>
       <c r="AI6" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="AJ6">
         <v>127</v>
       </c>
       <c r="AK6" t="s">
+        <v>582</v>
+      </c>
+      <c r="AL6" s="3" t="s">
+        <v>581</v>
+      </c>
+      <c r="AM6" t="s">
         <v>583</v>
-      </c>
-      <c r="AL6" s="3" t="s">
-        <v>582</v>
-      </c>
-      <c r="AM6" t="s">
-        <v>584</v>
       </c>
     </row>
   </sheetData>
@@ -5594,10 +5594,10 @@
         <v>225</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>227</v>
@@ -5618,13 +5618,13 @@
         <v>238</v>
       </c>
       <c r="O4" s="3" t="s">
+        <v>680</v>
+      </c>
+      <c r="P4" s="3" t="s">
         <v>681</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>682</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>683</v>
       </c>
       <c r="R4" s="3" t="s">
         <v>244</v>
@@ -5642,7 +5642,7 @@
         <v>255</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="X4" s="3" t="s">
         <v>262</v>
@@ -5654,7 +5654,7 @@
         <v>270</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="AB4" s="3" t="s">
         <v>277</v>
@@ -5730,109 +5730,109 @@
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>584</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>585</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>586</v>
       </c>
       <c r="D6">
         <v>9606</v>
       </c>
       <c r="E6" t="s">
+        <v>565</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>566</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>567</v>
-      </c>
       <c r="I6" s="3" t="s">
+        <v>570</v>
+      </c>
+      <c r="J6" s="3" t="s">
         <v>571</v>
       </c>
-      <c r="J6" s="3" t="s">
-        <v>572</v>
-      </c>
       <c r="K6" s="3" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="L6" t="s">
+        <v>586</v>
+      </c>
+      <c r="M6" t="s">
         <v>587</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
+        <v>586</v>
+      </c>
+      <c r="O6" t="s">
+        <v>661</v>
+      </c>
+      <c r="P6" t="s">
+        <v>662</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>661</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>659</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>660</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>659</v>
+      </c>
+      <c r="U6" t="s">
         <v>588</v>
       </c>
-      <c r="N6" t="s">
-        <v>587</v>
-      </c>
-      <c r="O6" t="s">
-        <v>662</v>
-      </c>
-      <c r="P6" t="s">
-        <v>663</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>662</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>660</v>
-      </c>
-      <c r="S6" s="3" t="s">
-        <v>661</v>
-      </c>
-      <c r="T6" s="3" t="s">
-        <v>660</v>
-      </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>589</v>
       </c>
-      <c r="V6" t="s">
+      <c r="W6" t="s">
         <v>590</v>
       </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>591</v>
-      </c>
-      <c r="X6" t="s">
-        <v>592</v>
       </c>
       <c r="Y6">
         <v>7200</v>
       </c>
       <c r="Z6" t="s">
+        <v>592</v>
+      </c>
+      <c r="AA6" t="s">
         <v>593</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>594</v>
       </c>
       <c r="AB6">
         <v>2400</v>
       </c>
       <c r="AC6" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="AD6">
         <v>5</v>
       </c>
       <c r="AE6" s="3" t="s">
+        <v>576</v>
+      </c>
+      <c r="AF6" s="3" t="s">
         <v>577</v>
       </c>
-      <c r="AF6" s="3" t="s">
+      <c r="AG6" s="3" t="s">
         <v>578</v>
       </c>
-      <c r="AG6" s="3" t="s">
-        <v>579</v>
-      </c>
       <c r="AH6" t="s">
+        <v>594</v>
+      </c>
+      <c r="AI6" t="s">
         <v>595</v>
       </c>
-      <c r="AI6" t="s">
-        <v>596</v>
-      </c>
       <c r="AJ6" s="3" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AK6" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
   </sheetData>
@@ -5940,13 +5940,13 @@
         <v>346</v>
       </c>
       <c r="Y1" s="1" t="s">
+        <v>696</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>697</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>698</v>
-      </c>
       <c r="AA1" s="1" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="2" spans="1:30" ht="119" x14ac:dyDescent="0.2">
@@ -6135,10 +6135,10 @@
         <v>305</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>705</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>706</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>707</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>309</v>
@@ -6177,25 +6177,25 @@
         <v>341</v>
       </c>
       <c r="U4" s="3" t="s">
+        <v>712</v>
+      </c>
+      <c r="V4" s="3" t="s">
         <v>713</v>
       </c>
-      <c r="V4" s="3" t="s">
+      <c r="W4" s="3" t="s">
         <v>714</v>
       </c>
-      <c r="W4" s="3" t="s">
-        <v>715</v>
-      </c>
       <c r="X4" s="3" t="s">
+        <v>671</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>694</v>
+      </c>
+      <c r="Z4" s="3" t="s">
+        <v>695</v>
+      </c>
+      <c r="AA4" s="3" t="s">
         <v>672</v>
-      </c>
-      <c r="Y4" s="3" t="s">
-        <v>695</v>
-      </c>
-      <c r="Z4" s="3" t="s">
-        <v>696</v>
-      </c>
-      <c r="AA4" s="3" t="s">
-        <v>673</v>
       </c>
       <c r="AB4" s="3" t="s">
         <v>220</v>
@@ -6243,67 +6243,67 @@
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
+        <v>596</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>597</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>598</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>599</v>
       </c>
       <c r="D6">
         <v>9606</v>
       </c>
       <c r="E6" t="s">
+        <v>565</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>566</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>567</v>
-      </c>
       <c r="I6" t="s">
+        <v>600</v>
+      </c>
+      <c r="J6" t="s">
         <v>601</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>602</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>603</v>
       </c>
-      <c r="L6" t="s">
-        <v>604</v>
-      </c>
       <c r="M6" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="N6">
         <v>98.7</v>
       </c>
       <c r="O6" t="s">
+        <v>604</v>
+      </c>
+      <c r="P6" t="s">
         <v>605</v>
-      </c>
-      <c r="P6" t="s">
-        <v>606</v>
       </c>
       <c r="Q6">
         <v>10</v>
       </c>
       <c r="R6" s="3" t="s">
+        <v>570</v>
+      </c>
+      <c r="S6" s="3" t="s">
         <v>571</v>
       </c>
-      <c r="S6" s="3" t="s">
-        <v>572</v>
-      </c>
       <c r="T6" s="3" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="U6" t="s">
+        <v>606</v>
+      </c>
+      <c r="V6" t="s">
         <v>607</v>
       </c>
-      <c r="V6" t="s">
-        <v>608</v>
-      </c>
       <c r="W6" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="X6">
         <v>1</v>
@@ -6312,19 +6312,19 @@
         <v>2217</v>
       </c>
       <c r="Z6" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="AA6" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="AB6" s="3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="AC6" s="3" t="s">
+        <v>628</v>
+      </c>
+      <c r="AD6" s="3" t="s">
         <v>629</v>
-      </c>
-      <c r="AD6" s="3" t="s">
-        <v>630</v>
       </c>
     </row>
   </sheetData>
@@ -6358,7 +6358,7 @@
         <v>355</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>357</v>
@@ -6382,22 +6382,22 @@
         <v>379</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>726</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>727</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>728</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>729</v>
-      </c>
       <c r="M1" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>731</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>732</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>733</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="85" x14ac:dyDescent="0.2">
@@ -6426,13 +6426,13 @@
         <v>380</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>718</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>719</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>720</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>721</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="119" x14ac:dyDescent="0.2">
@@ -6461,13 +6461,13 @@
         <v>381</v>
       </c>
       <c r="J3" s="2" t="s">
+        <v>724</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>725</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>726</v>
-      </c>
       <c r="L3" s="2" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
@@ -6478,7 +6478,7 @@
         <v>300</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>363</v>
@@ -6493,19 +6493,19 @@
         <v>375</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>382</v>
       </c>
       <c r="J4" s="3" t="s">
+        <v>721</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>722</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>723</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>724</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>435</v>
@@ -6514,7 +6514,7 @@
         <v>510</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -6538,16 +6538,16 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C6" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="E6" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -6556,19 +6556,19 @@
         <v>75</v>
       </c>
       <c r="J6" s="8" t="s">
+        <v>733</v>
+      </c>
+      <c r="K6" s="8" t="s">
         <v>734</v>
       </c>
-      <c r="K6" s="8" t="s">
-        <v>735</v>
-      </c>
       <c r="L6" s="8" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="O6">
         <v>1</v>
@@ -6576,16 +6576,16 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>610</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>596</v>
+      </c>
+      <c r="C7" t="s">
         <v>611</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>597</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="E7" s="3" t="s">
         <v>612</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>613</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -6594,19 +6594,19 @@
         <v>75</v>
       </c>
       <c r="J7" s="8" t="s">
+        <v>733</v>
+      </c>
+      <c r="K7" s="8" t="s">
         <v>734</v>
       </c>
-      <c r="K7" s="8" t="s">
-        <v>735</v>
-      </c>
       <c r="L7" s="8" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="O7">
         <v>1</v>
@@ -6754,13 +6754,13 @@
         <v>402</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>685</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>686</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>687</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>688</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -6778,31 +6778,31 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>615</v>
+      </c>
+      <c r="B6" t="s">
         <v>616</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>617</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>618</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>619</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>620</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>621</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>622</v>
       </c>
-      <c r="H6" t="s">
-        <v>623</v>
-      </c>
       <c r="I6" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dcp-967 managed access: add data use restriction and duos id attributes to template spreadsheet
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/current/not_accessioned_dcp_integration_test_metadata_1_SS2_bundle.xlsx
+++ b/infrastructure_testing_files/current/not_accessioned_dcp_integration_test_metadata_1_SS2_bundle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karoly/dev/hca/metadata-schema/infrastructure_testing_files/current/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexkoci/Documents/ebi-ait_github_repos HumanCellAtlas/metadata-schema/infrastructure_testing_files/current/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D224BAC-26DE-8544-A6DA-CD2F3478372D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45718CAF-5E73-8D4B-87F6-C825A10B9BCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="-5780" windowWidth="51200" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1100" yWindow="1680" windowWidth="33520" windowHeight="15880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1108" uniqueCount="745">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="749">
   <si>
     <t>PROJECT LABEL (Required)</t>
   </si>
@@ -2275,6 +2275,18 @@
   </si>
   <si>
     <t>SS2 1 Cell Integration Test without accessions</t>
+  </si>
+  <si>
+    <t>project.data_use_restriction</t>
+  </si>
+  <si>
+    <t>project.duos_id</t>
+  </si>
+  <si>
+    <t>GRU</t>
+  </si>
+  <si>
+    <t>DUOS-000108</t>
   </si>
 </sst>
 </file>
@@ -2354,7 +2366,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2362,11 +2374,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -2673,20 +2683,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="25.6640625" customWidth="1"/>
     <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="8" width="25.6640625" customWidth="1"/>
+    <col min="4" max="10" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2711,8 +2721,10 @@
       <c r="H1" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="85" x14ac:dyDescent="0.2">
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2737,8 +2749,10 @@
       <c r="H2" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="119" x14ac:dyDescent="0.2">
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" ht="119" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -2763,34 +2777,42 @@
       <c r="H3" s="2" t="s">
         <v>735</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" t="s">
         <v>667</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" t="s">
         <v>668</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" t="s">
         <v>669</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" t="s">
         <v>670</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I4" t="s">
+        <v>745</v>
+      </c>
+      <c r="J4" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -2801,8 +2823,10 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>744</v>
       </c>
@@ -2814,6 +2838,12 @@
       </c>
       <c r="D6" t="s">
         <v>535</v>
+      </c>
+      <c r="I6" t="s">
+        <v>747</v>
+      </c>
+      <c r="J6" t="s">
+        <v>748</v>
       </c>
     </row>
   </sheetData>
@@ -2925,31 +2955,31 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" t="s">
         <v>407</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>408</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
         <v>409</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" t="s">
         <v>410</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" t="s">
         <v>411</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" t="s">
         <v>412</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" t="s">
         <v>688</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" t="s">
         <v>689</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" t="s">
         <v>690</v>
       </c>
     </row>
@@ -3132,40 +3162,40 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" t="s">
         <v>416</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>417</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
         <v>418</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" t="s">
         <v>419</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" t="s">
         <v>420</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" t="s">
         <v>421</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" t="s">
         <v>707</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" t="s">
         <v>708</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" t="s">
         <v>709</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" t="s">
         <v>428</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" t="s">
         <v>710</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" t="s">
         <v>711</v>
       </c>
     </row>
@@ -3204,13 +3234,13 @@
       <c r="F6" t="s">
         <v>620</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" t="s">
         <v>633</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" t="s">
         <v>634</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" t="s">
         <v>635</v>
       </c>
       <c r="J6" t="s">
@@ -3546,100 +3576,100 @@
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" t="s">
         <v>435</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>436</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
         <v>437</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" t="s">
         <v>438</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" t="s">
         <v>439</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" t="s">
         <v>440</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" t="s">
         <v>444</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" t="s">
         <v>447</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" t="s">
         <v>451</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" t="s">
         <v>455</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" t="s">
         <v>458</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" t="s">
         <v>460</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="M4" t="s">
         <v>462</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="N4" t="s">
         <v>466</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="O4" t="s">
         <v>678</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="P4" t="s">
         <v>675</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="Q4" t="s">
         <v>674</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="R4" t="s">
         <v>471</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="S4" t="s">
         <v>475</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="T4" t="s">
         <v>479</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="U4" t="s">
         <v>483</v>
       </c>
-      <c r="V4" s="3" t="s">
+      <c r="V4" t="s">
         <v>487</v>
       </c>
-      <c r="W4" s="3" t="s">
+      <c r="W4" t="s">
         <v>491</v>
       </c>
-      <c r="X4" s="3" t="s">
+      <c r="X4" t="s">
         <v>492</v>
       </c>
-      <c r="Y4" s="3" t="s">
+      <c r="Y4" t="s">
         <v>493</v>
       </c>
-      <c r="Z4" s="3" t="s">
+      <c r="Z4" t="s">
         <v>494</v>
       </c>
-      <c r="AA4" s="3" t="s">
+      <c r="AA4" t="s">
         <v>495</v>
       </c>
-      <c r="AB4" s="3" t="s">
+      <c r="AB4" t="s">
         <v>496</v>
       </c>
-      <c r="AC4" s="3" t="s">
+      <c r="AC4" t="s">
         <v>497</v>
       </c>
-      <c r="AD4" s="3" t="s">
+      <c r="AD4" t="s">
         <v>501</v>
       </c>
-      <c r="AE4" s="3" t="s">
+      <c r="AE4" t="s">
         <v>505</v>
       </c>
-      <c r="AF4" s="3" t="s">
+      <c r="AF4" t="s">
         <v>509</v>
       </c>
     </row>
@@ -3698,40 +3728,39 @@
       <c r="F6" t="s">
         <v>620</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="K6" t="s">
         <v>639</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="L6" t="s">
         <v>640</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="M6" t="s">
         <v>639</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="N6" t="s">
         <v>641</v>
       </c>
-      <c r="O6" s="3" t="s">
+      <c r="O6" t="s">
         <v>642</v>
       </c>
-      <c r="P6" s="3" t="s">
+      <c r="P6" t="s">
         <v>643</v>
       </c>
-      <c r="Q6" s="3" t="s">
+      <c r="Q6" t="s">
         <v>642</v>
       </c>
-      <c r="R6" s="3" t="s">
+      <c r="R6" t="s">
         <v>644</v>
       </c>
       <c r="S6">
         <v>20014279</v>
       </c>
-      <c r="T6" s="3" t="s">
+      <c r="T6" t="s">
         <v>645</v>
       </c>
       <c r="U6" t="s">
         <v>646</v>
       </c>
-      <c r="V6" s="7"/>
       <c r="W6" t="s">
         <v>647</v>
       </c>
@@ -3747,17 +3776,17 @@
       <c r="AA6" t="s">
         <v>646</v>
       </c>
-      <c r="AB6" s="5"/>
+      <c r="AB6" s="4"/>
       <c r="AC6" t="s">
         <v>647</v>
       </c>
-      <c r="AD6" s="6" t="s">
+      <c r="AD6" s="5" t="s">
         <v>649</v>
       </c>
-      <c r="AE6" s="3" t="s">
+      <c r="AE6" t="s">
         <v>650</v>
       </c>
-      <c r="AF6" s="3" t="s">
+      <c r="AF6" t="s">
         <v>651</v>
       </c>
     </row>
@@ -3919,46 +3948,46 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" t="s">
         <v>510</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>511</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
         <v>512</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" t="s">
         <v>513</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" t="s">
         <v>514</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" t="s">
         <v>515</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" t="s">
         <v>518</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" t="s">
         <v>520</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" t="s">
         <v>522</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" t="s">
         <v>526</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" t="s">
         <v>530</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" t="s">
         <v>691</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="M4" t="s">
         <v>692</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="N4" t="s">
         <v>693</v>
       </c>
     </row>
@@ -3999,13 +4028,13 @@
       <c r="F6" t="s">
         <v>620</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" t="s">
         <v>654</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" t="s">
         <v>655</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" t="s">
         <v>654</v>
       </c>
       <c r="J6" t="s">
@@ -4014,13 +4043,13 @@
       <c r="K6" t="s">
         <v>550</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="L6" t="s">
         <v>657</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="M6" t="s">
         <v>658</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="N6" t="s">
         <v>657</v>
       </c>
     </row>
@@ -4141,34 +4170,34 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" t="s">
         <v>716</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" t="s">
         <v>45</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" t="s">
         <v>49</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" t="s">
         <v>53</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" t="s">
         <v>57</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" t="s">
         <v>700</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" t="s">
         <v>64</v>
       </c>
     </row>
@@ -4222,7 +4251,7 @@
       <c r="A7" t="s">
         <v>538</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>540</v>
       </c>
       <c r="C7" t="s">
@@ -4334,22 +4363,22 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>698</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
         <v>75</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" t="s">
         <v>79</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" t="s">
         <v>699</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" t="s">
         <v>740</v>
       </c>
     </row>
@@ -4376,7 +4405,7 @@
       <c r="D6">
         <v>27565351</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>558</v>
       </c>
       <c r="F6" t="s">
@@ -4438,13 +4467,13 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" t="s">
         <v>86</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>90</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
         <v>666</v>
       </c>
     </row>
@@ -4922,136 +4951,136 @@
       </c>
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" t="s">
         <v>96</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>99</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
         <v>102</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" t="s">
         <v>106</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" t="s">
         <v>110</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" t="s">
         <v>113</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" t="s">
         <v>701</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" t="s">
         <v>702</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" t="s">
         <v>123</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" t="s">
         <v>126</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" t="s">
         <v>129</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" t="s">
         <v>132</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="M4" t="s">
         <v>135</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="N4" t="s">
         <v>137</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="O4" t="s">
         <v>139</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="P4" t="s">
         <v>143</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="Q4" t="s">
         <v>147</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="R4" t="s">
         <v>151</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="S4" t="s">
         <v>154</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="T4" t="s">
         <v>156</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="U4" t="s">
         <v>158</v>
       </c>
-      <c r="V4" s="3" t="s">
+      <c r="V4" t="s">
         <v>161</v>
       </c>
-      <c r="W4" s="3" t="s">
+      <c r="W4" t="s">
         <v>163</v>
       </c>
-      <c r="X4" s="3" t="s">
+      <c r="X4" t="s">
         <v>165</v>
       </c>
-      <c r="Y4" s="3" t="s">
+      <c r="Y4" t="s">
         <v>168</v>
       </c>
-      <c r="Z4" s="3" t="s">
+      <c r="Z4" t="s">
         <v>171</v>
       </c>
-      <c r="AA4" s="3" t="s">
+      <c r="AA4" t="s">
         <v>173</v>
       </c>
-      <c r="AB4" s="3" t="s">
+      <c r="AB4" t="s">
         <v>177</v>
       </c>
-      <c r="AC4" s="3" t="s">
+      <c r="AC4" t="s">
         <v>179</v>
       </c>
-      <c r="AD4" s="3" t="s">
+      <c r="AD4" t="s">
         <v>181</v>
       </c>
-      <c r="AE4" s="3" t="s">
+      <c r="AE4" t="s">
         <v>183</v>
       </c>
-      <c r="AF4" s="3" t="s">
+      <c r="AF4" t="s">
         <v>187</v>
       </c>
-      <c r="AG4" s="3" t="s">
+      <c r="AG4" t="s">
         <v>190</v>
       </c>
-      <c r="AH4" s="3" t="s">
+      <c r="AH4" t="s">
         <v>192</v>
       </c>
-      <c r="AI4" s="3" t="s">
+      <c r="AI4" t="s">
         <v>194</v>
       </c>
-      <c r="AJ4" s="3" t="s">
+      <c r="AJ4" t="s">
         <v>198</v>
       </c>
-      <c r="AK4" s="3" t="s">
+      <c r="AK4" t="s">
         <v>201</v>
       </c>
-      <c r="AL4" s="3" t="s">
+      <c r="AL4" t="s">
         <v>203</v>
       </c>
-      <c r="AM4" s="3" t="s">
+      <c r="AM4" t="s">
         <v>205</v>
       </c>
-      <c r="AN4" s="3" t="s">
+      <c r="AN4" t="s">
         <v>209</v>
       </c>
-      <c r="AO4" s="3" t="s">
+      <c r="AO4" t="s">
         <v>211</v>
       </c>
-      <c r="AP4" s="3" t="s">
+      <c r="AP4" t="s">
         <v>213</v>
       </c>
-      <c r="AQ4" s="3" t="s">
+      <c r="AQ4" t="s">
         <v>215</v>
       </c>
-      <c r="AR4" s="3" t="s">
+      <c r="AR4" t="s">
         <v>219</v>
       </c>
     </row>
@@ -5125,22 +5154,22 @@
       <c r="I6">
         <v>36.4</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="J6" t="s">
         <v>567</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="K6" t="s">
         <v>568</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="L6" t="s">
         <v>569</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="M6" t="s">
         <v>570</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="N6" t="s">
         <v>571</v>
       </c>
-      <c r="O6" s="3" t="s">
+      <c r="O6" t="s">
         <v>570</v>
       </c>
       <c r="P6" t="s">
@@ -5152,13 +5181,13 @@
       <c r="R6" t="s">
         <v>573</v>
       </c>
-      <c r="S6" s="3" t="s">
+      <c r="S6" t="s">
         <v>574</v>
       </c>
-      <c r="T6" s="3" t="s">
+      <c r="T6" t="s">
         <v>575</v>
       </c>
-      <c r="U6" s="3" t="s">
+      <c r="U6" t="s">
         <v>574</v>
       </c>
       <c r="V6" t="s">
@@ -5185,7 +5214,7 @@
       <c r="AC6" t="s">
         <v>576</v>
       </c>
-      <c r="AD6" s="3" t="s">
+      <c r="AD6" t="s">
         <v>577</v>
       </c>
       <c r="AE6" t="s">
@@ -5209,7 +5238,7 @@
       <c r="AK6" t="s">
         <v>582</v>
       </c>
-      <c r="AL6" s="3" t="s">
+      <c r="AL6" t="s">
         <v>581</v>
       </c>
       <c r="AM6" t="s">
@@ -5575,115 +5604,115 @@
       <c r="AK3" s="2"/>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" t="s">
         <v>220</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>221</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
         <v>222</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" t="s">
         <v>223</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" t="s">
         <v>224</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" t="s">
         <v>225</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" t="s">
         <v>704</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" t="s">
         <v>703</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" t="s">
         <v>227</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" t="s">
         <v>229</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" t="s">
         <v>231</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" t="s">
         <v>233</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="M4" t="s">
         <v>236</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="N4" t="s">
         <v>238</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="O4" t="s">
         <v>680</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="P4" t="s">
         <v>681</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="Q4" t="s">
         <v>682</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="R4" t="s">
         <v>244</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="S4" t="s">
         <v>246</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="T4" t="s">
         <v>248</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="U4" t="s">
         <v>252</v>
       </c>
-      <c r="V4" s="3" t="s">
+      <c r="V4" t="s">
         <v>255</v>
       </c>
-      <c r="W4" s="3" t="s">
+      <c r="W4" t="s">
         <v>683</v>
       </c>
-      <c r="X4" s="3" t="s">
+      <c r="X4" t="s">
         <v>262</v>
       </c>
-      <c r="Y4" s="3" t="s">
+      <c r="Y4" t="s">
         <v>266</v>
       </c>
-      <c r="Z4" s="3" t="s">
+      <c r="Z4" t="s">
         <v>270</v>
       </c>
-      <c r="AA4" s="3" t="s">
+      <c r="AA4" t="s">
         <v>684</v>
       </c>
-      <c r="AB4" s="3" t="s">
+      <c r="AB4" t="s">
         <v>277</v>
       </c>
-      <c r="AC4" s="3" t="s">
+      <c r="AC4" t="s">
         <v>281</v>
       </c>
-      <c r="AD4" s="3" t="s">
+      <c r="AD4" t="s">
         <v>285</v>
       </c>
-      <c r="AE4" s="3" t="s">
+      <c r="AE4" t="s">
         <v>287</v>
       </c>
-      <c r="AF4" s="3" t="s">
+      <c r="AF4" t="s">
         <v>289</v>
       </c>
-      <c r="AG4" s="3" t="s">
+      <c r="AG4" t="s">
         <v>291</v>
       </c>
-      <c r="AH4" s="3" t="s">
+      <c r="AH4" t="s">
         <v>295</v>
       </c>
-      <c r="AI4" s="3" t="s">
+      <c r="AI4" t="s">
         <v>299</v>
       </c>
-      <c r="AJ4" s="3" t="s">
+      <c r="AJ4" t="s">
         <v>96</v>
       </c>
-      <c r="AK4" s="3" t="s">
+      <c r="AK4" t="s">
         <v>385</v>
       </c>
     </row>
@@ -5732,10 +5761,10 @@
       <c r="A6" t="s">
         <v>599</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
         <v>584</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" t="s">
         <v>585</v>
       </c>
       <c r="D6">
@@ -5744,16 +5773,16 @@
       <c r="E6" t="s">
         <v>565</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" t="s">
         <v>566</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" t="s">
         <v>570</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="J6" t="s">
         <v>571</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="K6" t="s">
         <v>570</v>
       </c>
       <c r="L6" t="s">
@@ -5774,13 +5803,13 @@
       <c r="Q6" t="s">
         <v>661</v>
       </c>
-      <c r="R6" s="3" t="s">
+      <c r="R6" t="s">
         <v>659</v>
       </c>
-      <c r="S6" s="3" t="s">
+      <c r="S6" t="s">
         <v>660</v>
       </c>
-      <c r="T6" s="3" t="s">
+      <c r="T6" t="s">
         <v>659</v>
       </c>
       <c r="U6" t="s">
@@ -5813,13 +5842,13 @@
       <c r="AD6">
         <v>5</v>
       </c>
-      <c r="AE6" s="3" t="s">
+      <c r="AE6" t="s">
         <v>576</v>
       </c>
-      <c r="AF6" s="3" t="s">
+      <c r="AF6" t="s">
         <v>577</v>
       </c>
-      <c r="AG6" s="3" t="s">
+      <c r="AG6" t="s">
         <v>578</v>
       </c>
       <c r="AH6" t="s">
@@ -5828,10 +5857,10 @@
       <c r="AI6" t="s">
         <v>595</v>
       </c>
-      <c r="AJ6" s="3" t="s">
+      <c r="AJ6" t="s">
         <v>562</v>
       </c>
-      <c r="AK6" s="3" t="s">
+      <c r="AK6" t="s">
         <v>615</v>
       </c>
     </row>
@@ -6116,94 +6145,94 @@
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" t="s">
         <v>300</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>301</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
         <v>302</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" t="s">
         <v>303</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" t="s">
         <v>304</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" t="s">
         <v>305</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" t="s">
         <v>705</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" t="s">
         <v>706</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" t="s">
         <v>309</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" t="s">
         <v>313</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" t="s">
         <v>315</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" t="s">
         <v>317</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="M4" t="s">
         <v>319</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="N4" t="s">
         <v>323</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="O4" t="s">
         <v>327</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="P4" t="s">
         <v>331</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="Q4" t="s">
         <v>335</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="R4" t="s">
         <v>337</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="S4" t="s">
         <v>339</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="T4" t="s">
         <v>341</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="U4" t="s">
         <v>712</v>
       </c>
-      <c r="V4" s="3" t="s">
+      <c r="V4" t="s">
         <v>713</v>
       </c>
-      <c r="W4" s="3" t="s">
+      <c r="W4" t="s">
         <v>714</v>
       </c>
-      <c r="X4" s="3" t="s">
+      <c r="X4" t="s">
         <v>671</v>
       </c>
-      <c r="Y4" s="3" t="s">
+      <c r="Y4" t="s">
         <v>694</v>
       </c>
-      <c r="Z4" s="3" t="s">
+      <c r="Z4" t="s">
         <v>695</v>
       </c>
-      <c r="AA4" s="3" t="s">
+      <c r="AA4" t="s">
         <v>672</v>
       </c>
-      <c r="AB4" s="3" t="s">
+      <c r="AB4" t="s">
         <v>220</v>
       </c>
-      <c r="AC4" s="3" t="s">
+      <c r="AC4" t="s">
         <v>407</v>
       </c>
-      <c r="AD4" s="3" t="s">
+      <c r="AD4" t="s">
         <v>416</v>
       </c>
     </row>
@@ -6242,13 +6271,13 @@
       <c r="AD5" s="1"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" t="s">
         <v>596</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
         <v>597</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" t="s">
         <v>598</v>
       </c>
       <c r="D6">
@@ -6257,7 +6286,7 @@
       <c r="E6" t="s">
         <v>565</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" t="s">
         <v>566</v>
       </c>
       <c r="I6" t="s">
@@ -6287,13 +6316,13 @@
       <c r="Q6">
         <v>10</v>
       </c>
-      <c r="R6" s="3" t="s">
+      <c r="R6" t="s">
         <v>570</v>
       </c>
-      <c r="S6" s="3" t="s">
+      <c r="S6" t="s">
         <v>571</v>
       </c>
-      <c r="T6" s="3" t="s">
+      <c r="T6" t="s">
         <v>570</v>
       </c>
       <c r="U6" t="s">
@@ -6317,13 +6346,13 @@
       <c r="AA6" t="s">
         <v>663</v>
       </c>
-      <c r="AB6" s="3" t="s">
+      <c r="AB6" t="s">
         <v>599</v>
       </c>
-      <c r="AC6" s="3" t="s">
+      <c r="AC6" t="s">
         <v>628</v>
       </c>
-      <c r="AD6" s="3" t="s">
+      <c r="AD6" t="s">
         <v>629</v>
       </c>
     </row>
@@ -6334,7 +6363,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:Q11"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
@@ -6345,15 +6374,15 @@
     <col min="1" max="1" width="25.6640625" customWidth="1"/>
     <col min="2" max="2" width="25.83203125" customWidth="1"/>
     <col min="3" max="9" width="25.6640625" customWidth="1"/>
-    <col min="10" max="10" width="24" style="3" customWidth="1"/>
-    <col min="11" max="11" width="31.33203125" style="3" customWidth="1"/>
-    <col min="12" max="12" width="37.1640625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="24" customWidth="1"/>
+    <col min="11" max="11" width="31.33203125" customWidth="1"/>
+    <col min="12" max="12" width="37.1640625" customWidth="1"/>
     <col min="13" max="13" width="33.83203125" customWidth="1"/>
     <col min="14" max="14" width="24.1640625" customWidth="1"/>
     <col min="15" max="15" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>355</v>
       </c>
@@ -6400,7 +6429,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="85" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>356</v>
       </c>
@@ -6435,7 +6464,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="119" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="119" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>82</v>
       </c>
@@ -6470,54 +6499,54 @@
         <v>724</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>362</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>300</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
         <v>715</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" t="s">
         <v>363</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" t="s">
         <v>367</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" t="s">
         <v>371</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" t="s">
         <v>375</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" t="s">
         <v>717</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" t="s">
         <v>382</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" t="s">
         <v>721</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" t="s">
         <v>722</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" t="s">
         <v>723</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="M4" t="s">
         <v>435</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="N4" t="s">
         <v>510</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="O4" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -6536,11 +6565,11 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>609</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
         <v>596</v>
       </c>
       <c r="C6" t="s">
@@ -6552,79 +6581,65 @@
       <c r="F6">
         <v>1</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6">
         <v>75</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="J6" s="6" t="s">
         <v>733</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="K6" s="6" t="s">
         <v>734</v>
       </c>
-      <c r="L6" s="8" t="s">
+      <c r="L6" s="6" t="s">
         <v>733</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="M6" t="s">
         <v>636</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="N6" t="s">
         <v>613</v>
       </c>
       <c r="O6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>610</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" t="s">
         <v>596</v>
       </c>
       <c r="C7" t="s">
         <v>611</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" t="s">
         <v>612</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7">
         <v>75</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="J7" s="6" t="s">
         <v>733</v>
       </c>
-      <c r="K7" s="8" t="s">
+      <c r="K7" s="6" t="s">
         <v>734</v>
       </c>
-      <c r="L7" s="8" t="s">
+      <c r="L7" s="6" t="s">
         <v>733</v>
       </c>
-      <c r="M7" s="3" t="s">
+      <c r="M7" t="s">
         <v>636</v>
       </c>
-      <c r="N7" s="3" t="s">
+      <c r="N7" t="s">
         <v>613</v>
       </c>
       <c r="O7">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6735,31 +6750,31 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" t="s">
         <v>385</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>388</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
         <v>391</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" t="s">
         <v>394</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" t="s">
         <v>398</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" t="s">
         <v>402</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" t="s">
         <v>685</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" t="s">
         <v>686</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" t="s">
         <v>687</v>
       </c>
     </row>

</xml_diff>